<commit_message>
fix: 修正 SERVER 到 QA 的 games 表遊戲 minBet 錯誤，重新計算 coin size 設定
</commit_message>
<xml_diff>
--- a/input/gameMinBet.xlsx
+++ b/input/gameMinBet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\chiisen\coin_size\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9027850C-1485-4323-A280-CC6466D44E93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FB9CCED-8541-4374-B87B-D5C98FBCA746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -378,7 +378,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -388,6 +388,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -421,12 +427,15 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -815,8 +824,8 @@
   </sheetPr>
   <dimension ref="A1:D106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A77" sqref="A77:XFD77"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A106" sqref="A106:XFD106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.375" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1551,8 +1560,8 @@
       <c r="C52" t="s">
         <v>58</v>
       </c>
-      <c r="D52">
-        <v>5</v>
+      <c r="D52" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1565,8 +1574,8 @@
       <c r="C53" t="s">
         <v>59</v>
       </c>
-      <c r="D53">
-        <v>50</v>
+      <c r="D53" s="2">
+        <v>40</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1579,8 +1588,8 @@
       <c r="C54" t="s">
         <v>60</v>
       </c>
-      <c r="D54">
-        <v>50</v>
+      <c r="D54" s="2">
+        <v>30</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1593,8 +1602,8 @@
       <c r="C55" t="s">
         <v>61</v>
       </c>
-      <c r="D55">
-        <v>50</v>
+      <c r="D55" s="2">
+        <v>25</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1621,8 +1630,8 @@
       <c r="C57" t="s">
         <v>63</v>
       </c>
-      <c r="D57">
-        <v>50</v>
+      <c r="D57" s="2">
+        <v>30</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1649,8 +1658,8 @@
       <c r="C59" t="s">
         <v>65</v>
       </c>
-      <c r="D59">
-        <v>50</v>
+      <c r="D59" s="2">
+        <v>20</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1663,8 +1672,8 @@
       <c r="C60" t="s">
         <v>66</v>
       </c>
-      <c r="D60">
-        <v>50</v>
+      <c r="D60" s="2">
+        <v>30</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1677,8 +1686,8 @@
       <c r="C61" t="s">
         <v>67</v>
       </c>
-      <c r="D61">
-        <v>50</v>
+      <c r="D61" s="2">
+        <v>20</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2195,8 +2204,8 @@
       <c r="C98" t="s">
         <v>100</v>
       </c>
-      <c r="D98">
-        <v>30</v>
+      <c r="D98" s="2">
+        <v>25</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2223,8 +2232,8 @@
       <c r="C100" t="s">
         <v>101</v>
       </c>
-      <c r="D100">
-        <v>1</v>
+      <c r="D100" s="2">
+        <v>10</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2237,8 +2246,8 @@
       <c r="C101" t="s">
         <v>102</v>
       </c>
-      <c r="D101">
-        <v>1</v>
+      <c r="D101" s="2">
+        <v>3</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>